<commit_message>
planing for next module
</commit_message>
<xml_diff>
--- a/daily work schedule.xlsx
+++ b/daily work schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Project Plan</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Check style.css file</t>
+  </si>
+  <si>
+    <t>Meeting5</t>
+  </si>
+  <si>
+    <t>All Member</t>
+  </si>
+  <si>
+    <t>Planing for next module</t>
+  </si>
+  <si>
+    <t>DOM manipulating</t>
   </si>
 </sst>
 </file>
@@ -423,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,6 +448,7 @@
     <col min="3" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
     <col min="11" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -589,6 +602,30 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
planing for next day
</commit_message>
<xml_diff>
--- a/daily work schedule.xlsx
+++ b/daily work schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Project Plan</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>DOM manipulating</t>
+  </si>
+  <si>
+    <t>Meeting6</t>
+  </si>
+  <si>
+    <t>Set Condition with DOM and Frontend</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,6 +455,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
     <col min="11" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,6 +633,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update per days work's plan
</commit_message>
<xml_diff>
--- a/daily work schedule.xlsx
+++ b/daily work schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Project Plan</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>Set Condition with DOM and Frontend</t>
+  </si>
+  <si>
+    <t>Meeting 7</t>
+  </si>
+  <si>
+    <t>All Members</t>
+  </si>
+  <si>
+    <t>Problem sloving Session</t>
+  </si>
+  <si>
+    <t>Work with functionality</t>
   </si>
 </sst>
 </file>
@@ -441,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,6 +468,7 @@
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
     <col min="11" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -633,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
@@ -641,11 +654,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reschedule all works for all days
</commit_message>
<xml_diff>
--- a/daily work schedule.xlsx
+++ b/daily work schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Project Plan</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Meeting2</t>
   </si>
   <si>
-    <t>All member</t>
-  </si>
-  <si>
     <t>Manage the frontend(html page)</t>
   </si>
   <si>
@@ -74,18 +71,12 @@
     <t>Meeting4</t>
   </si>
   <si>
-    <t>All  Member</t>
-  </si>
-  <si>
     <t>Check style.css file</t>
   </si>
   <si>
     <t>Meeting5</t>
   </si>
   <si>
-    <t>All Member</t>
-  </si>
-  <si>
     <t>Planing for next module</t>
   </si>
   <si>
@@ -104,10 +95,55 @@
     <t>All Members</t>
   </si>
   <si>
-    <t>Problem sloving Session</t>
-  </si>
-  <si>
     <t>Work with functionality</t>
+  </si>
+  <si>
+    <t>Finish the JavaScript All Activity</t>
+  </si>
+  <si>
+    <t>Make ER and Class Diagram</t>
+  </si>
+  <si>
+    <t>Edit Readme File And Add all Important topic</t>
+  </si>
+  <si>
+    <t>Check All Work</t>
+  </si>
+  <si>
+    <t>All  Members</t>
+  </si>
+  <si>
+    <t>All members</t>
+  </si>
+  <si>
+    <t>Final Check HTML File</t>
+  </si>
+  <si>
+    <t>Final Check CSS File</t>
+  </si>
+  <si>
+    <t>沙姆</t>
+  </si>
+  <si>
+    <t>Final Check JS File</t>
+  </si>
+  <si>
+    <t>大山</t>
+  </si>
+  <si>
+    <t>Final Check All File</t>
+  </si>
+  <si>
+    <t>Final Check All Works</t>
+  </si>
+  <si>
+    <t>Final Meeting</t>
+  </si>
+  <si>
+    <t>Final Problem Solving Session</t>
+  </si>
+  <si>
+    <t>Problem solving Session</t>
   </si>
 </sst>
 </file>
@@ -453,23 +489,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" customWidth="1"/>
-    <col min="11" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.45">
@@ -538,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -554,20 +594,20 @@
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -575,23 +615,23 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
@@ -599,24 +639,24 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>3</v>
@@ -624,66 +664,160 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="I19" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="I21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="J22" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="J23" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="K24" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>3</v>
+      <c r="L25" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="18:18" x14ac:dyDescent="0.3">
+      <c r="R33" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>